<commit_message>
Fixed bug from hard-coded row index in ExcelWriter
</commit_message>
<xml_diff>
--- a/testoutput.xlsx
+++ b/testoutput.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Worksheet1" sheetId="1" r:id="Rebf39f959f3c43cc"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Worksheet1" sheetId="1" r:id="Rdd36b03941f84023"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -57,7 +57,7 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>keyword</x:t>
+            <x:t>keyword1</x:t>
           </x:r>
         </x:is>
       </x:c>
@@ -65,7 +65,7 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>file1</x:t>
+            <x:t>MultiplePresentationsMultipleKeywords1.pptx</x:t>
           </x:r>
         </x:is>
       </x:c>
@@ -73,7 +73,7 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>1,2,3</x:t>
+            <x:t>1,2</x:t>
           </x:r>
         </x:is>
       </x:c>
@@ -81,17 +81,17 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>path/file1</x:t>
-          </x:r>
-        </x:is>
-      </x:c>
-    </x:row>
-    <x:row r="2">
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\MultiplePresentationsMultipleKeywords1.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="3">
       <x:c r="A3" t="inlineStr">
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>keyword</x:t>
+            <x:t>keyword1</x:t>
           </x:r>
         </x:is>
       </x:c>
@@ -99,7 +99,7 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>file2</x:t>
+            <x:t>MultiplePresentationsMultipleKeywords2.pptx</x:t>
           </x:r>
         </x:is>
       </x:c>
@@ -107,7 +107,7 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>1,2,3</x:t>
+            <x:t>1,2</x:t>
           </x:r>
         </x:is>
       </x:c>
@@ -115,7 +115,279 @@
         <x:is>
           <x:r>
             <x:rPr/>
-            <x:t>path/file2</x:t>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\MultiplePresentationsMultipleKeywords2.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="4">
+      <x:c r="A4" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>keyword1</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B4" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>NewlineBetweenKeywords.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C4" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>1</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D4" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\NewlineBetweenKeywords.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="5">
+      <x:c r="A5" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>keyword2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B5" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>MultiplePresentationsMultipleKeywords1.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C5" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D5" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\MultiplePresentationsMultipleKeywords1.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="6">
+      <x:c r="A6" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>keyword2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B6" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>MultiplePresentationsMultipleKeywords2.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C6" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D6" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\MultiplePresentationsMultipleKeywords2.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="7">
+      <x:c r="A7" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>keyword2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B7" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>NewlineBetweenKeywords.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C7" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>1</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D7" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\NewlineBetweenKeywords.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="8">
+      <x:c r="A8" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>mykeyword</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B8" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>BulletPointKeyword.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C8" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D8" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\BulletPointKeyword.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="9">
+      <x:c r="A9" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>mykeyword</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B9" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>LowercaseKeywordPrefix.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C9" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>1</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D9" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\LowercaseKeywordPrefix.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="10">
+      <x:c r="A10" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>mykeyword</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B10" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>SingleKeyword.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C10" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>1</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D10" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\SingleKeyword.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+    </x:row>
+    <x:row r="11">
+      <x:c r="A11" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>mykeyword</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="B11" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>TextboxKeyword.pptx</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="C11" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>2</x:t>
+          </x:r>
+        </x:is>
+      </x:c>
+      <x:c r="D11" t="inlineStr">
+        <x:is>
+          <x:r>
+            <x:rPr/>
+            <x:t>C:\Users\rober\source\repos\PptKeywordReader\TestFiles\TextboxKeyword.pptx</x:t>
           </x:r>
         </x:is>
       </x:c>

</xml_diff>